<commit_message>
some changes in azubihandler
</commit_message>
<xml_diff>
--- a/src/main/resources/Gradingtable.xlsx
+++ b/src/main/resources/Gradingtable.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="103">
   <si>
     <t>Datum:</t>
   </si>
@@ -5512,7 +5512,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -5564,6 +5564,17 @@
         <v>7.0</v>
       </c>
       <c r="C4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C5" t="s">
         <v>102</v>
       </c>
     </row>

</xml_diff>